<commit_message>
updated Value and Record management cheat sheet
Also fixed Doxygen error in ValueArchive.h
</commit_message>
<xml_diff>
--- a/Developer Notes/Value and record management 07142016.xlsx
+++ b/Developer Notes/Value and record management 07142016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>Value Storage and Record Management</t>
   </si>
@@ -44,7 +44,127 @@
     <t>For record keeping across timesteps, The RecordMgr class is used. The RecordMgr can either store records in memory, or write them to disk (the default behavior). When disk writing is enabled, RecordMgr writes out binary .omet files containing all the values for a submodel at a specific time. There are two types of records: full and diffs. A full record is a snapshot, while a diff is a record of just the values that changed between steps. Diff records take up less space, while full records do not require walking across multiple files. The RecordMgr will write out full records on an interval defined by RM_KEYFRAME_INT, and will write out diff records for each intermediate timestep. Finally, there are two record keeping modes: full record and partial. Full record records anything value at a given point, while partial recording only records values for items that utilize previous value lookups. Use the full record if you will be parsing timesteps at the end of a run; use partials if you are only concerned with the final timestep.</t>
   </si>
   <si>
-    <t>&lt;&lt;TODO ADD table of important functions&gt;&gt;</t>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Relevant Methods &amp; classes</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>AddEvaluable</t>
+  </si>
+  <si>
+    <t>AddSpaceForEvaluable</t>
+  </si>
+  <si>
+    <t>AddSpaceForModel</t>
+  </si>
+  <si>
+    <t>AllocSpaceForModel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetIDValPairs </t>
+  </si>
+  <si>
+    <t>IndexForID</t>
+  </si>
+  <si>
+    <t>RecordState</t>
+  </si>
+  <si>
+    <t>ValueArchive</t>
+  </si>
+  <si>
+    <t>SingleValForTime</t>
+  </si>
+  <si>
+    <t>CacheRecord</t>
+  </si>
+  <si>
+    <t>SyncArchiveWithCache</t>
+  </si>
+  <si>
+    <t>RecordMgr</t>
+  </si>
+  <si>
+    <t>GetArchiveIndex</t>
+  </si>
+  <si>
+    <t>GetValueArchive</t>
+  </si>
+  <si>
+    <t>SetCurrentInstance</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>GetModelIndex</t>
+  </si>
+  <si>
+    <t>GetValue</t>
+  </si>
+  <si>
+    <t>SetValue</t>
+  </si>
+  <si>
+    <t>Evaluable</t>
+  </si>
+  <si>
+    <t>Retrieves the Index from an Evaluable object used to locate partition in ValueArchive</t>
+  </si>
+  <si>
+    <t>Retrieve associated value from ValueArchive</t>
+  </si>
+  <si>
+    <t>Set the associated value in the ValueArchive</t>
+  </si>
+  <si>
+    <t>Set the submodel instance to act upon when any contained Evaluables query the ValueArchive. Basically the current instance is used as an offset applied to the model index of an Evaluable object.</t>
+  </si>
+  <si>
+    <t>Retrieve pointer to the associated value archive</t>
+  </si>
+  <si>
+    <t>Get the ValueArchive index for a modelIndex after it is transformed by the current Model instance/state</t>
+  </si>
+  <si>
+    <t>Copy Cached record into ValueArchive.</t>
+  </si>
+  <si>
+    <t>Record the current values in the ValueArchive according to the present RecordMgr settings</t>
+  </si>
+  <si>
+    <t>Retrieve a record from storage and place into memory.</t>
+  </si>
+  <si>
+    <t>Retrieve a specific value from a previously saved record.</t>
+  </si>
+  <si>
+    <t>Inform the associated RecordMgr to record the current values in the ValueArchive.</t>
+  </si>
+  <si>
+    <t>Retrieve the ValueArchive index for a specific object ID.</t>
+  </si>
+  <si>
+    <t>Returns a container of ID-value tuples.</t>
+  </si>
+  <si>
+    <t>Allocate a enough space for all components in a submodel to store their values.</t>
+  </si>
+  <si>
+    <t>Expand the space for all subcomponents for a given submodel. This can be useful when dynamically adding instances.</t>
+  </si>
+  <si>
+    <t>Expand space for a an Evaluable object if more is needed.</t>
+  </si>
+  <si>
+    <t>Allocate space for an Evaluable object in the ValueArchive</t>
   </si>
 </sst>
 </file>
@@ -68,21 +188,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,17 +204,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,20 +261,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -155,7 +294,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6705600" y="571500"/>
+          <a:off x="6029325" y="771525"/>
           <a:ext cx="6667500" cy="3638550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -441,144 +580,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -589,143 +738,377 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A5:J13"/>
-    <mergeCell ref="A17:J27"/>
+    <mergeCell ref="A5:C14"/>
+    <mergeCell ref="A17:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>